<commit_message>
RQ2 cifar results updated
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -176,7 +176,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -185,6 +184,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,22 +487,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -515,7 +515,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
@@ -528,10 +528,10 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -546,7 +546,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="2"/>
@@ -556,17 +556,17 @@
       <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -600,10 +600,10 @@
       <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -628,10 +628,10 @@
       <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>